<commit_message>
Added time plots and FINALLY figured out captions <3 captioner
</commit_message>
<xml_diff>
--- a/chapters/price_data.xlsx
+++ b/chapters/price_data.xlsx
@@ -2868,13 +2868,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>10.019622</v>
+        <v>9.960678</v>
       </c>
       <c r="C2" t="n">
-        <v>0.043059039056539516</v>
+        <v>0.043058962224881814</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0421577794564576</v>
+        <v>0.042157705796523004</v>
       </c>
     </row>
     <row r="3">
@@ -2882,13 +2882,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>10.457878</v>
+        <v>10.396358</v>
       </c>
       <c r="C3" t="n">
-        <v>0.04373977381581873</v>
+        <v>0.04373999440600307</v>
       </c>
       <c r="D3" t="n">
-        <v>0.042810199593201315</v>
+        <v>0.042810410939138954</v>
       </c>
     </row>
     <row r="4">
@@ -2896,13 +2896,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>11.145187</v>
+        <v>11.079622</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0657216502238791</v>
+        <v>0.06572147669405015</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0636521755342212</v>
+        <v>0.06365201270573495</v>
       </c>
     </row>
     <row r="5">
@@ -2910,13 +2910,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>11.12242</v>
+        <v>11.056989</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.002042765186443085</v>
+        <v>-0.0020427592204860234</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0020448544770181876</v>
+        <v>-0.0020448484988491167</v>
       </c>
     </row>
     <row r="6">
@@ -2924,13 +2924,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>11.023804</v>
+        <v>10.958953</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.008866415762037727</v>
+        <v>-0.008866428283504924</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.008905956321809683</v>
+        <v>-0.00890596895529061</v>
       </c>
     </row>
     <row r="7">
@@ -2938,13 +2938,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>11.389889</v>
+        <v>11.322885</v>
       </c>
       <c r="C7" t="n">
-        <v>0.033208591154197054</v>
+        <v>0.03320864684792424</v>
       </c>
       <c r="D7" t="n">
-        <v>0.03266909729808409</v>
+        <v>0.032669151201745183</v>
       </c>
     </row>
     <row r="8">
@@ -2952,13 +2952,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>11.52876</v>
+        <v>11.460938</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01219248054129407</v>
+        <v>0.012192387364174717</v>
       </c>
       <c r="D8" t="n">
-        <v>0.012118750943230339</v>
+        <v>0.012118658888482514</v>
       </c>
     </row>
     <row r="9">
@@ -2966,13 +2966,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>11.467941</v>
+        <v>11.400478</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.005275415569410802</v>
+        <v>-0.005275309926639937</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.005289379706862274</v>
+        <v>-0.005289273503831904</v>
       </c>
     </row>
     <row r="10">
@@ -2980,13 +2980,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>11.129411</v>
+        <v>11.063939</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.02951968448390163</v>
+        <v>-0.029519727155299713</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.02996415940607866</v>
+        <v>-0.029964203375439258</v>
       </c>
     </row>
     <row r="11">
@@ -2994,13 +2994,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>11.492519</v>
+        <v>11.424911</v>
       </c>
       <c r="C11" t="n">
-        <v>0.03262598532842409</v>
+        <v>0.032625993328415426</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0321050580978004</v>
+        <v>0.03210506584503081</v>
       </c>
     </row>
     <row r="12">
@@ -3008,13 +3008,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>12.04096</v>
+        <v>11.970125</v>
       </c>
       <c r="C12" t="n">
-        <v>0.047721565655014286</v>
+        <v>0.04772150960300725</v>
       </c>
       <c r="D12" t="n">
-        <v>0.04661786897233977</v>
+        <v>0.04661781547338517</v>
       </c>
     </row>
     <row r="13">
@@ -3022,13 +3022,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>11.971475</v>
+        <v>11.901049</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.005770719278197278</v>
+        <v>-0.005770699971805127</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.005787434214513887</v>
+        <v>-0.005787414796063484</v>
       </c>
     </row>
     <row r="14">
@@ -3036,13 +3036,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>12.514196</v>
+        <v>12.440578</v>
       </c>
       <c r="C14" t="n">
-        <v>0.04533451391745813</v>
+        <v>0.04533457512862937</v>
       </c>
       <c r="D14" t="n">
-        <v>0.044336943204737356</v>
+        <v>0.04433700176127475</v>
       </c>
     </row>
     <row r="15">
@@ -3050,13 +3050,13 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>12.445875</v>
+        <v>12.372659</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.005459479778005538</v>
+        <v>-0.0054594730244847955</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.005474437202406257</v>
+        <v>-0.005474430411812392</v>
       </c>
     </row>
     <row r="16">
@@ -3064,13 +3064,13 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>12.34151</v>
+        <v>12.268908</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.00838550925507442</v>
+        <v>-0.008385505492392475</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.008420865429566327</v>
+        <v>-0.008420861635065613</v>
       </c>
     </row>
     <row r="17">
@@ -3078,13 +3078,13 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>12.466915</v>
+        <v>12.393576</v>
       </c>
       <c r="C17" t="n">
-        <v>0.010161236347902225</v>
+        <v>0.010161295528501757</v>
       </c>
       <c r="D17" t="n">
-        <v>0.010109958060485535</v>
+        <v>0.01011001664578437</v>
       </c>
     </row>
     <row r="18">
@@ -3092,13 +3092,13 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>12.489008</v>
+        <v>12.415538</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0017721304749411804</v>
+        <v>0.0017720470669644328</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0017705621043626607</v>
+        <v>0.0017704788439307784</v>
       </c>
     </row>
     <row r="19">
@@ -3106,13 +3106,13 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>12.36104</v>
+        <v>12.288323</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.010246450318552425</v>
+        <v>-0.010246434749746625</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.010299306559845345</v>
+        <v>-0.01029929082986314</v>
       </c>
     </row>
     <row r="20">
@@ -3120,13 +3120,13 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>12.064152</v>
+        <v>11.993181</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.024018043789195365</v>
+        <v>-0.024018086113133608</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.024311180228870022</v>
+        <v>-0.02431122359436344</v>
       </c>
     </row>
     <row r="21">
@@ -3134,13 +3134,13 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>12.179894</v>
+        <v>12.108243</v>
       </c>
       <c r="C21" t="n">
-        <v>0.00959387779596943</v>
+        <v>0.009593951763089192</v>
       </c>
       <c r="D21" t="n">
-        <v>0.00954814879669641</v>
+        <v>0.009548222060925315</v>
       </c>
     </row>
     <row r="22">
@@ -3148,13 +3148,13 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>12.163423</v>
+        <v>12.091868</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.0013523106194521795</v>
+        <v>-0.0013523844871629054</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.001353225816638215</v>
+        <v>-0.0013532997843790362</v>
       </c>
     </row>
     <row r="23">
@@ -3162,13 +3162,13 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>12.614856</v>
+        <v>12.540646</v>
       </c>
       <c r="C23" t="n">
-        <v>0.037113976879699084</v>
+        <v>0.03711403399375501</v>
       </c>
       <c r="D23" t="n">
-        <v>0.036441833409923685</v>
+        <v>0.036441888480104545</v>
       </c>
     </row>
     <row r="24">
@@ -3176,13 +3176,13 @@
         <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>11.952927</v>
+        <v>11.88261</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.05247218041965773</v>
+        <v>-0.05247225701132141</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.0538989814219204</v>
+        <v>-0.05389906225507923</v>
       </c>
     </row>
     <row r="25">
@@ -3190,13 +3190,13 @@
         <v>26</v>
       </c>
       <c r="B25" t="n">
-        <v>11.402876</v>
+        <v>11.335795</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.04601810083839708</v>
+        <v>-0.046018088618578035</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.04711058133900625</v>
+        <v>-0.047110568529728614</v>
       </c>
     </row>
     <row r="26">
@@ -3204,13 +3204,13 @@
         <v>27</v>
       </c>
       <c r="B26" t="n">
-        <v>11.373879</v>
+        <v>11.306969</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.0025429549527681283</v>
+        <v>-0.002542918251432602</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.002546193754630721</v>
+        <v>-0.002546156959728041</v>
       </c>
     </row>
     <row r="27">
@@ -3218,13 +3218,13 @@
         <v>28</v>
       </c>
       <c r="B27" t="n">
-        <v>11.202539</v>
+        <v>11.136638</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.015064341725456898</v>
+        <v>-0.015064249313852307</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.015178961492280596</v>
+        <v>-0.015178867667268392</v>
       </c>
     </row>
     <row r="28">
@@ -3232,13 +3232,13 @@
         <v>29</v>
       </c>
       <c r="B28" t="n">
-        <v>11.288216</v>
+        <v>11.221809</v>
       </c>
       <c r="C28" t="n">
-        <v>0.007647998368941034</v>
+        <v>0.0076478197459595165</v>
       </c>
       <c r="D28" t="n">
-        <v>0.00761890069455573</v>
+        <v>0.007618723427297969</v>
       </c>
     </row>
     <row r="29">
@@ -3246,13 +3246,13 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>11.519367</v>
+        <v>11.451601</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02047719497926015</v>
+        <v>0.02047726886101886</v>
       </c>
       <c r="D29" t="n">
-        <v>0.020270356108963217</v>
+        <v>0.020270428508186278</v>
       </c>
     </row>
     <row r="30">
@@ -3260,13 +3260,13 @@
         <v>31</v>
       </c>
       <c r="B30" t="n">
-        <v>11.336215</v>
+        <v>11.269526</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.015899484754674953</v>
+        <v>-0.015899523568800422</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.016027237507244774</v>
+        <v>-0.016027276948466174</v>
       </c>
     </row>
     <row r="31">
@@ -3274,13 +3274,13 @@
         <v>32</v>
       </c>
       <c r="B31" t="n">
-        <v>11.235028</v>
+        <v>11.168935</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.008925995140353304</v>
+        <v>-0.008925929981438818</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.00896607048811715</v>
+        <v>-0.008966004742358535</v>
       </c>
     </row>
     <row r="32">
@@ -3288,13 +3288,13 @@
         <v>33</v>
       </c>
       <c r="B32" t="n">
-        <v>11.767722</v>
+        <v>11.698495</v>
       </c>
       <c r="C32" t="n">
-        <v>0.04741367800774543</v>
+        <v>0.04741365224168659</v>
       </c>
       <c r="D32" t="n">
-        <v>0.04632396178862308</v>
+        <v>0.046323937188926134</v>
       </c>
     </row>
     <row r="33">
@@ -3302,13 +3302,13 @@
         <v>34</v>
       </c>
       <c r="B33" t="n">
-        <v>11.934204</v>
+        <v>11.863997</v>
       </c>
       <c r="C33" t="n">
-        <v>0.014147343045663341</v>
+        <v>0.0141472898864341</v>
       </c>
       <c r="D33" t="n">
-        <v>0.014048203336235243</v>
+        <v>0.014048150918575253</v>
       </c>
     </row>
     <row r="34">
@@ -3316,13 +3316,13 @@
         <v>35</v>
       </c>
       <c r="B34" t="n">
-        <v>12.014527</v>
+        <v>11.943849</v>
       </c>
       <c r="C34" t="n">
-        <v>0.006730486591313589</v>
+        <v>0.006730615322980915</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0067079379852854615</v>
+        <v>0.006708065856310341</v>
       </c>
     </row>
     <row r="35">
@@ -3330,13 +3330,13 @@
         <v>36</v>
       </c>
       <c r="B35" t="n">
-        <v>12.267352</v>
+        <v>12.195186</v>
       </c>
       <c r="C35" t="n">
-        <v>0.02104327536156858</v>
+        <v>0.0210432164706702</v>
       </c>
       <c r="D35" t="n">
-        <v>0.020824923555178287</v>
+        <v>0.020824865877995258</v>
       </c>
     </row>
     <row r="36">
@@ -3344,13 +3344,13 @@
         <v>37</v>
       </c>
       <c r="B36" t="n">
-        <v>12.576908</v>
+        <v>12.50292</v>
       </c>
       <c r="C36" t="n">
-        <v>0.025234133658184943</v>
+        <v>0.025234055470740868</v>
       </c>
       <c r="D36" t="n">
-        <v>0.02492100958694765</v>
+        <v>0.02492093332393175</v>
       </c>
     </row>
     <row r="37">
@@ -3358,13 +3358,13 @@
         <v>38</v>
       </c>
       <c r="B37" t="n">
-        <v>12.591887</v>
+        <v>12.517813</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0011909922534218964</v>
+        <v>0.0011911617446163092</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0011902835847714677</v>
+        <v>0.001190452874328951</v>
       </c>
     </row>
     <row r="38">
@@ -3372,13 +3372,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="n">
-        <v>12.635395</v>
+        <v>12.561063</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0034552406640877553</v>
+        <v>0.0034550763779586102</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0034492850348764037</v>
+        <v>0.003449121314427206</v>
       </c>
     </row>
     <row r="39">
@@ -3386,13 +3386,13 @@
         <v>40</v>
       </c>
       <c r="B39" t="n">
-        <v>13.078058</v>
+        <v>13.001122</v>
       </c>
       <c r="C39" t="n">
-        <v>0.03503357037908228</v>
+        <v>0.035033579562493866</v>
       </c>
       <c r="D39" t="n">
-        <v>0.03443386134019599</v>
+        <v>0.03443387021276978</v>
       </c>
     </row>
     <row r="40">
@@ -3400,13 +3400,13 @@
         <v>41</v>
       </c>
       <c r="B40" t="n">
-        <v>12.747569</v>
+        <v>12.672578</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.025270495053623554</v>
+        <v>-0.02527043435174292</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.025595277299569563</v>
+        <v>-0.02559521502395512</v>
       </c>
     </row>
     <row r="41">
@@ -3414,13 +3414,13 @@
         <v>42</v>
       </c>
       <c r="B41" t="n">
-        <v>13.006311</v>
+        <v>12.929798</v>
       </c>
       <c r="C41" t="n">
-        <v>0.020297360226094963</v>
+        <v>0.020297369643335283</v>
       </c>
       <c r="D41" t="n">
-        <v>0.02009411444309972</v>
+        <v>0.020094123672997455</v>
       </c>
     </row>
     <row r="42">
@@ -3428,13 +3428,13 @@
         <v>43</v>
       </c>
       <c r="B42" t="n">
-        <v>13.245667</v>
+        <v>13.167747</v>
       </c>
       <c r="C42" t="n">
-        <v>0.018403066019257786</v>
+        <v>0.018403149066984925</v>
       </c>
       <c r="D42" t="n">
-        <v>0.01823577888030803</v>
+        <v>0.01823586042731673</v>
       </c>
     </row>
     <row r="43">
@@ -3442,13 +3442,13 @@
         <v>44</v>
       </c>
       <c r="B43" t="n">
-        <v>13.451762</v>
+        <v>13.372629</v>
       </c>
       <c r="C43" t="n">
-        <v>0.015559427849122232</v>
+        <v>0.015559381570742437</v>
       </c>
       <c r="D43" t="n">
-        <v>0.015439621103106038</v>
+        <v>0.015439575533758187</v>
       </c>
     </row>
     <row r="44">
@@ -3456,13 +3456,13 @@
         <v>45</v>
       </c>
       <c r="B44" t="n">
-        <v>14.344801</v>
+        <v>14.260413</v>
       </c>
       <c r="C44" t="n">
-        <v>0.06638825456471809</v>
+        <v>0.06638814252605107</v>
       </c>
       <c r="D44" t="n">
-        <v>0.06427747572260456</v>
+        <v>0.06427737065892591</v>
       </c>
     </row>
     <row r="45">
@@ -3470,13 +3470,13 @@
         <v>46</v>
       </c>
       <c r="B45" t="n">
-        <v>13.826604</v>
+        <v>13.745265</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.036124377047823786</v>
+        <v>-0.03612433945636806</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.03679301452946637</v>
+        <v>-0.036792975529149174</v>
       </c>
     </row>
     <row r="46">
@@ -3484,13 +3484,13 @@
         <v>47</v>
       </c>
       <c r="B46" t="n">
-        <v>13.903795</v>
+        <v>13.822002</v>
       </c>
       <c r="C46" t="n">
-        <v>0.005582788080138901</v>
+        <v>0.005582795238942229</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0055672620775490955</v>
+        <v>0.0055672691966082155</v>
       </c>
     </row>
     <row r="47">
@@ -3498,13 +3498,13 @@
         <v>48</v>
       </c>
       <c r="B47" t="n">
-        <v>13.575157</v>
+        <v>13.495298</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.023636568289448823</v>
+        <v>-0.023636518067353784</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.023920393325116862</v>
+        <v>-0.023920341887207375</v>
       </c>
     </row>
     <row r="48">
@@ -3512,13 +3512,13 @@
         <v>49</v>
       </c>
       <c r="B48" t="n">
-        <v>13.284714</v>
+        <v>13.206562</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.021395185337451328</v>
+        <v>-0.021395303756908457</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.021627380189749523</v>
+        <v>-0.02162750119821233</v>
       </c>
     </row>
     <row r="49">
@@ -3526,13 +3526,13 @@
         <v>50</v>
       </c>
       <c r="B49" t="n">
-        <v>12.819459</v>
+        <v>12.744045</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.03502183035329176</v>
+        <v>-0.035021756608570875</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.03564980002679885</v>
+        <v>-0.03564972360567298</v>
       </c>
     </row>
     <row r="50">
@@ -3540,13 +3540,13 @@
         <v>51</v>
       </c>
       <c r="B50" t="n">
-        <v>13.163469</v>
+        <v>13.086032</v>
       </c>
       <c r="C50" t="n">
-        <v>0.026834985782161258</v>
+        <v>0.02683504334769693</v>
       </c>
       <c r="D50" t="n">
-        <v>0.02648124206991831</v>
+        <v>0.02648129813105271</v>
       </c>
     </row>
     <row r="51">
@@ -3554,13 +3554,13 @@
         <v>52</v>
       </c>
       <c r="B51" t="n">
-        <v>12.96734</v>
+        <v>12.891056</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.014899491919645125</v>
+        <v>-0.014899550910466908</v>
       </c>
       <c r="D51" t="n">
-        <v>-0.015011604355379404</v>
+        <v>-0.015011664238429923</v>
       </c>
     </row>
     <row r="52">
@@ -3568,13 +3568,13 @@
         <v>53</v>
       </c>
       <c r="B52" t="n">
-        <v>13.117543</v>
+        <v>13.040376</v>
       </c>
       <c r="C52" t="n">
-        <v>0.011583177428832636</v>
+        <v>0.011583224834334604</v>
       </c>
       <c r="D52" t="n">
-        <v>0.01151660600836868</v>
+        <v>0.011516652871050859</v>
       </c>
     </row>
     <row r="53">
@@ -3582,13 +3582,13 @@
         <v>54</v>
       </c>
       <c r="B53" t="n">
-        <v>13.191799</v>
+        <v>13.114195</v>
       </c>
       <c r="C53" t="n">
-        <v>0.005660816206205954</v>
+        <v>0.00566080303206018</v>
       </c>
       <c r="D53" t="n">
-        <v>0.005644853997234911</v>
+        <v>0.0056448408972458175</v>
       </c>
     </row>
     <row r="54">
@@ -3596,13 +3596,13 @@
         <v>55</v>
       </c>
       <c r="B54" t="n">
-        <v>13.127671</v>
+        <v>13.050445</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.004861202024075695</v>
+        <v>-0.004861144736676648</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.004873056098940065</v>
+        <v>-0.004872998531696648</v>
       </c>
     </row>
     <row r="55">
@@ -3610,13 +3610,13 @@
         <v>56</v>
       </c>
       <c r="B55" t="n">
-        <v>12.987808</v>
+        <v>12.911404</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.010654060419399647</v>
+        <v>-0.010654119457229383</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.010711221280476746</v>
+        <v>-0.010711280954074365</v>
       </c>
     </row>
     <row r="56">
@@ -3624,13 +3624,13 @@
         <v>57</v>
       </c>
       <c r="B56" t="n">
-        <v>13.289283</v>
+        <v>13.211105</v>
       </c>
       <c r="C56" t="n">
-        <v>0.023212154044777833</v>
+        <v>0.02321211542912005</v>
       </c>
       <c r="D56" t="n">
-        <v>0.02294684967635119</v>
+        <v>0.022946811936710887</v>
       </c>
     </row>
     <row r="57">
@@ -3638,13 +3638,13 @@
         <v>58</v>
       </c>
       <c r="B57" t="n">
-        <v>13.549207</v>
+        <v>13.4695</v>
       </c>
       <c r="C57" t="n">
-        <v>0.019558918265191405</v>
+        <v>0.019558924102109243</v>
       </c>
       <c r="D57" t="n">
-        <v>0.019370100696693093</v>
+        <v>0.019370106421637168</v>
       </c>
     </row>
     <row r="58">
@@ -3652,13 +3652,13 @@
         <v>59</v>
       </c>
       <c r="B58" t="n">
-        <v>13.951736</v>
+        <v>13.869662</v>
       </c>
       <c r="C58" t="n">
-        <v>0.029708675939484896</v>
+        <v>0.029708749396785583</v>
       </c>
       <c r="D58" t="n">
-        <v>0.029275923341376853</v>
+        <v>0.029275994679319073</v>
       </c>
     </row>
     <row r="59">
@@ -3666,13 +3666,13 @@
         <v>60</v>
       </c>
       <c r="B59" t="n">
-        <v>14.134841</v>
+        <v>14.051689</v>
       </c>
       <c r="C59" t="n">
-        <v>0.013124173221167545</v>
+        <v>0.013124112180959768</v>
       </c>
       <c r="D59" t="n">
-        <v>0.013038797439529848</v>
+        <v>0.013038737190044891</v>
       </c>
     </row>
     <row r="60">
@@ -3680,13 +3680,13 @@
         <v>61</v>
       </c>
       <c r="B60" t="n">
-        <v>14.15</v>
+        <v>14.066758</v>
       </c>
       <c r="C60" t="n">
-        <v>0.001072456350941886</v>
+        <v>0.0010723977736770696</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0010718816804655695</v>
+        <v>0.001071823165953223</v>
       </c>
     </row>
     <row r="61">
@@ -3694,13 +3694,13 @@
         <v>62</v>
       </c>
       <c r="B61" t="n">
-        <v>14.83</v>
+        <v>14.785746</v>
       </c>
       <c r="C61" t="n">
-        <v>0.048056537102473484</v>
+        <v>0.05111255912698587</v>
       </c>
       <c r="D61" t="n">
-        <v>0.046937532060594034</v>
+        <v>0.04984918333157351</v>
       </c>
     </row>
   </sheetData>
@@ -3733,13 +3733,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>9.911574</v>
+        <v>9.888234</v>
       </c>
       <c r="C2" t="n">
-        <v>0.008112029738548854</v>
+        <v>0.008112215894029884</v>
       </c>
       <c r="D2" t="n">
-        <v>0.008079304087156292</v>
+        <v>0.00807948874467268</v>
       </c>
     </row>
     <row r="3">
@@ -3747,13 +3747,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>9.945006</v>
+        <v>9.921587</v>
       </c>
       <c r="C3" t="n">
-        <v>0.003373026322559536</v>
+        <v>0.0033729986567878623</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0033673504289843947</v>
+        <v>0.003367322856215882</v>
       </c>
     </row>
     <row r="4">
@@ -3761,13 +3761,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>9.92179</v>
+        <v>9.898425</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0023344380083829552</v>
+        <v>-0.00233450555843584</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0023371670568139713</v>
+        <v>-0.00233723476492953</v>
       </c>
     </row>
     <row r="5">
@@ -3775,13 +3775,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>9.954425</v>
+        <v>9.930984</v>
       </c>
       <c r="C5" t="n">
-        <v>0.003289225028951348</v>
+        <v>0.0032893111782936746</v>
       </c>
       <c r="D5" t="n">
-        <v>0.003283827361163283</v>
+        <v>0.0032839132280662042</v>
       </c>
     </row>
     <row r="6">
@@ -3789,13 +3789,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>9.930209</v>
+        <v>9.906824</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.002432686970869846</v>
+        <v>-0.002432790144460739</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0024356507614444745</v>
+        <v>-0.00243575418664177</v>
       </c>
     </row>
     <row r="7">
@@ -3803,13 +3803,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>9.96212</v>
+        <v>9.938661</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0032135275299847166</v>
+        <v>0.003213643444155201</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0032083751855744858</v>
+        <v>0.003208490728438207</v>
       </c>
     </row>
     <row r="8">
@@ -3817,13 +3817,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>10.022242</v>
+        <v>9.998641</v>
       </c>
       <c r="C8" t="n">
-        <v>0.006035060810349435</v>
+        <v>0.0060350181981252415</v>
       </c>
       <c r="D8" t="n">
-        <v>0.006016922770389677</v>
+        <v>0.006016880413789227</v>
       </c>
     </row>
     <row r="9">
@@ -3831,13 +3831,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>10.015676</v>
+        <v>9.99209</v>
       </c>
       <c r="C9" t="n">
-        <v>-6.551428313146257E-4</v>
+        <v>-6.551890401905736E-4</v>
       </c>
       <c r="D9" t="n">
-        <v>-6.553575311571969E-4</v>
+        <v>-6.554037703274673E-4</v>
       </c>
     </row>
     <row r="10">
@@ -3845,13 +3845,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>10.004393</v>
+        <v>9.980834</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0011265340452304429</v>
+        <v>-0.0011264910544239726</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0011271690616645458</v>
+        <v>-0.0011271260223737478</v>
       </c>
     </row>
     <row r="11">
@@ -3859,13 +3859,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>10.044953</v>
+        <v>10.021299</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0040542189816010765</v>
+        <v>0.004054270414676875</v>
       </c>
       <c r="D11" t="n">
-        <v>0.004046022781151848</v>
+        <v>0.004046074006547329</v>
       </c>
     </row>
     <row r="12">
@@ -3873,13 +3873,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>10.058201</v>
+        <v>10.034515</v>
       </c>
       <c r="C12" t="n">
-        <v>0.001318871277944167</v>
+        <v>0.0013187911068215374</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0013180023311556432</v>
+        <v>0.0013179222656258816</v>
       </c>
     </row>
     <row r="13">
@@ -3887,13 +3887,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>10.061051</v>
+        <v>10.037359</v>
       </c>
       <c r="C13" t="n">
-        <v>2.8335086960407097E-4</v>
+        <v>2.834217697615937E-4</v>
       </c>
       <c r="D13" t="n">
-        <v>2.833107333279905E-4</v>
+        <v>2.8338161339913626E-4</v>
       </c>
     </row>
     <row r="14">
@@ -3901,13 +3901,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>10.111241</v>
+        <v>10.087431</v>
       </c>
       <c r="C14" t="n">
-        <v>0.004988544437355413</v>
+        <v>0.004988563226641318</v>
       </c>
       <c r="D14" t="n">
-        <v>0.004976142876279344</v>
+        <v>0.004976161572299187</v>
       </c>
     </row>
     <row r="15">
@@ -3915,13 +3915,13 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>10.123587</v>
+        <v>10.099748</v>
       </c>
       <c r="C15" t="n">
-        <v>0.001221017281656911</v>
+        <v>0.001221024461034892</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0012202724462988535</v>
+        <v>0.0012202796169211716</v>
       </c>
     </row>
     <row r="16">
@@ -3929,13 +3929,13 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>10.144485</v>
+        <v>10.120595</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0020642880828702914</v>
+        <v>0.0020641109065293595</v>
       </c>
       <c r="D16" t="n">
-        <v>0.002062160367866994</v>
+        <v>0.0020619835565001132</v>
       </c>
     </row>
     <row r="17">
@@ -3943,13 +3943,13 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>10.136909</v>
+        <v>10.113037</v>
       </c>
       <c r="C17" t="n">
-        <v>-7.468097197639301E-4</v>
+        <v>-7.467940373068194E-4</v>
       </c>
       <c r="D17" t="n">
-        <v>-7.470887210585531E-4</v>
+        <v>-7.470730268810399E-4</v>
       </c>
     </row>
     <row r="18">
@@ -3957,13 +3957,13 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>10.157843</v>
+        <v>10.133922</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0020651265587963152</v>
+        <v>0.002065156095048426</v>
       </c>
       <c r="D18" t="n">
-        <v>0.002062997116152765</v>
+        <v>0.002063026591534012</v>
       </c>
     </row>
     <row r="19">
@@ -3971,13 +3971,13 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>10.157906</v>
+        <v>10.133985</v>
       </c>
       <c r="C19" t="n">
-        <v>6.202104128050223E-6</v>
+        <v>6.216744119269535E-6</v>
       </c>
       <c r="D19" t="n">
-        <v>6.202084894990634E-6</v>
+        <v>6.216724795393702E-6</v>
       </c>
     </row>
     <row r="20">
@@ -3985,13 +3985,13 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>10.150273</v>
+        <v>10.12637</v>
       </c>
       <c r="C20" t="n">
-        <v>-7.514343999643902E-4</v>
+        <v>-7.514319391630497E-4</v>
       </c>
       <c r="D20" t="n">
-        <v>-7.517168683062181E-4</v>
+        <v>-7.517144056543579E-4</v>
       </c>
     </row>
     <row r="21">
@@ -3999,13 +3999,13 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>10.169415</v>
+        <v>10.145468</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0018858606069023232</v>
+        <v>0.0018859670345838797</v>
       </c>
       <c r="D21" t="n">
-        <v>0.001884084604299563</v>
+        <v>0.0018841908316455935</v>
       </c>
     </row>
     <row r="22">
@@ -4013,13 +4013,13 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>10.177089</v>
+        <v>10.153123</v>
       </c>
       <c r="C22" t="n">
-        <v>7.54615678483006E-4</v>
+        <v>7.545240889825777E-4</v>
       </c>
       <c r="D22" t="n">
-        <v>7.543310992281782E-4</v>
+        <v>7.542395787862866E-4</v>
       </c>
     </row>
     <row r="23">
@@ -4027,13 +4027,13 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>10.205874</v>
+        <v>10.181841</v>
       </c>
       <c r="C23" t="n">
-        <v>0.00282841193586858</v>
+        <v>0.0028284893229404418</v>
       </c>
       <c r="D23" t="n">
-        <v>0.00282441950521628</v>
+        <v>0.0028244966740200717</v>
       </c>
     </row>
     <row r="24">
@@ -4041,13 +4041,13 @@
         <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>10.157878</v>
+        <v>10.133958</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.004702781946945067</v>
+        <v>-0.004702784103582158</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.004713874817864561</v>
+        <v>-0.004713876984691723</v>
       </c>
     </row>
     <row r="25">
@@ -4055,13 +4055,13 @@
         <v>26</v>
       </c>
       <c r="B25" t="n">
-        <v>10.099264</v>
+        <v>10.075481</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.005770299662980816</v>
+        <v>-0.00577040086410463</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.005787012163850136</v>
+        <v>-0.005787113952329115</v>
       </c>
     </row>
     <row r="26">
@@ -4069,13 +4069,13 @@
         <v>27</v>
       </c>
       <c r="B26" t="n">
-        <v>10.127165</v>
+        <v>10.103316</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0027626765673220977</v>
+        <v>0.002762647262199991</v>
       </c>
       <c r="D26" t="n">
-        <v>0.002758867390483921</v>
+        <v>0.002758838166098787</v>
       </c>
     </row>
     <row r="27">
@@ -4083,13 +4083,13 @@
         <v>28</v>
       </c>
       <c r="B27" t="n">
-        <v>10.097329</v>
+        <v>10.073551</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.0029461354683172347</v>
+        <v>-0.0029460624610769814</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.0029504838681662093</v>
+        <v>-0.002950410645203849</v>
       </c>
     </row>
     <row r="28">
@@ -4097,13 +4097,13 @@
         <v>29</v>
       </c>
       <c r="B28" t="n">
-        <v>10.154182</v>
+        <v>10.130271</v>
       </c>
       <c r="C28" t="n">
-        <v>0.00563049891709011</v>
+        <v>0.0056305864734294</v>
       </c>
       <c r="D28" t="n">
-        <v>0.005614706908257716</v>
+        <v>0.005614793974367593</v>
       </c>
     </row>
     <row r="29">
@@ -4111,13 +4111,13 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>10.191799</v>
+        <v>10.167798</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0037045820135976903</v>
+        <v>0.0037044418653753297</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0036977369498414348</v>
+        <v>0.0036975973188835276</v>
       </c>
     </row>
     <row r="30">
@@ -4125,13 +4125,13 @@
         <v>31</v>
       </c>
       <c r="B30" t="n">
-        <v>10.200484</v>
+        <v>10.176463</v>
       </c>
       <c r="C30" t="n">
-        <v>8.521557381573341E-4</v>
+        <v>8.522002502411308E-4</v>
       </c>
       <c r="D30" t="n">
-        <v>8.51792859594358E-4</v>
+        <v>8.518373337782492E-4</v>
       </c>
     </row>
     <row r="31">
@@ -4139,13 +4139,13 @@
         <v>32</v>
       </c>
       <c r="B31" t="n">
-        <v>10.164757</v>
+        <v>10.140821</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.0035024808626726855</v>
+        <v>-0.0035023956751965013</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.0035086289085759503</v>
+        <v>-0.0035085434216872713</v>
       </c>
     </row>
     <row r="32">
@@ -4153,13 +4153,13 @@
         <v>33</v>
       </c>
       <c r="B32" t="n">
-        <v>10.212254</v>
+        <v>10.188205</v>
       </c>
       <c r="C32" t="n">
-        <v>0.004672713769743764</v>
+        <v>0.004672599979823833</v>
       </c>
       <c r="D32" t="n">
-        <v>0.004661830532423306</v>
+        <v>0.004661717271731813</v>
       </c>
     </row>
     <row r="33">
@@ -4167,13 +4167,13 @@
         <v>34</v>
       </c>
       <c r="B33" t="n">
-        <v>10.230688</v>
+        <v>10.206596</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0018050863208067813</v>
+        <v>0.0018051266145509004</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0018034591103699427</v>
+        <v>0.001803499331510583</v>
       </c>
     </row>
     <row r="34">
@@ -4181,13 +4181,13 @@
         <v>35</v>
       </c>
       <c r="B34" t="n">
-        <v>10.203534</v>
+        <v>10.179506</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.0026541714496625124</v>
+        <v>-0.0026541659922660887</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.00265770000768617</v>
+        <v>-0.002657694535766364</v>
       </c>
     </row>
     <row r="35">
@@ -4195,13 +4195,13 @@
         <v>36</v>
       </c>
       <c r="B35" t="n">
-        <v>10.231731</v>
+        <v>10.207638</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0027634543090662156</v>
+        <v>0.0027635918678174942</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0027596429891980634</v>
+        <v>0.0027597801688501455</v>
       </c>
     </row>
     <row r="36">
@@ -4209,13 +4209,13 @@
         <v>37</v>
       </c>
       <c r="B36" t="n">
-        <v>10.270645</v>
+        <v>10.246459</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0038032665245011366</v>
+        <v>0.003803132517042229</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0037960523920994582</v>
+        <v>0.0037959188923668563</v>
       </c>
     </row>
     <row r="37">
@@ -4223,13 +4223,13 @@
         <v>38</v>
       </c>
       <c r="B37" t="n">
-        <v>10.260918</v>
+        <v>10.236755</v>
       </c>
       <c r="C37" t="n">
-        <v>-9.470680760556016E-4</v>
+        <v>-9.470588815118086E-4</v>
       </c>
       <c r="D37" t="n">
-        <v>-9.47516828381012E-4</v>
+        <v>-9.475076251210801E-4</v>
       </c>
     </row>
     <row r="38">
@@ -4237,13 +4237,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="n">
-        <v>10.241439</v>
+        <v>10.217321</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.0018983681577030564</v>
+        <v>-0.0018984531719282716</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.001900172342233386</v>
+        <v>-0.0019002575181574777</v>
       </c>
     </row>
     <row r="39">
@@ -4251,13 +4251,13 @@
         <v>40</v>
       </c>
       <c r="B39" t="n">
-        <v>10.27071</v>
+        <v>10.246524</v>
       </c>
       <c r="C39" t="n">
-        <v>0.002858094453328075</v>
+        <v>0.0028581856241967074</v>
       </c>
       <c r="D39" t="n">
-        <v>0.002854017867041314</v>
+        <v>0.00285410877807335</v>
       </c>
     </row>
     <row r="40">
@@ -4265,13 +4265,13 @@
         <v>41</v>
       </c>
       <c r="B40" t="n">
-        <v>10.251193</v>
+        <v>10.227053</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.0019002581126326135</v>
+        <v>-0.0019002541740011925</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.0019020658936099721</v>
+        <v>-0.0019020619474798828</v>
       </c>
     </row>
     <row r="41">
@@ -4279,13 +4279,13 @@
         <v>42</v>
       </c>
       <c r="B41" t="n">
-        <v>10.300064</v>
+        <v>10.275808</v>
       </c>
       <c r="C41" t="n">
-        <v>0.0047673475662786124</v>
+        <v>0.0047672579774449275</v>
       </c>
       <c r="D41" t="n">
-        <v>0.004756019753018315</v>
+        <v>0.004755930589255275</v>
       </c>
     </row>
     <row r="42">
@@ -4293,13 +4293,13 @@
         <v>43</v>
       </c>
       <c r="B42" t="n">
-        <v>10.319645</v>
+        <v>10.295344</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0019010561487771138</v>
+        <v>0.0019011643658581878</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0018992514284246198</v>
+        <v>0.001899359440163284</v>
       </c>
     </row>
     <row r="43">
@@ -4307,13 +4307,13 @@
         <v>44</v>
       </c>
       <c r="B43" t="n">
-        <v>10.283443</v>
+        <v>10.259228</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.003508066411199273</v>
+        <v>-0.0035079935162921627</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.003514234104849301</v>
+        <v>-0.0035141609533244633</v>
       </c>
     </row>
     <row r="44">
@@ -4321,13 +4321,13 @@
         <v>45</v>
       </c>
       <c r="B44" t="n">
-        <v>10.391409</v>
+        <v>10.366939</v>
       </c>
       <c r="C44" t="n">
-        <v>0.010499012830625043</v>
+        <v>0.01049893812672864</v>
       </c>
       <c r="D44" t="n">
-        <v>0.01044428094926042</v>
+        <v>0.010444207021529373</v>
       </c>
     </row>
     <row r="45">
@@ -4335,13 +4335,13 @@
         <v>46</v>
       </c>
       <c r="B45" t="n">
-        <v>10.341334</v>
+        <v>10.316982</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.004818884522782341</v>
+        <v>-0.004818876623080559</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.004830532782950758</v>
+        <v>-0.0048305248449969085</v>
       </c>
     </row>
     <row r="46">
@@ -4349,13 +4349,13 @@
         <v>47</v>
       </c>
       <c r="B46" t="n">
-        <v>10.384618</v>
+        <v>10.360164</v>
       </c>
       <c r="C46" t="n">
-        <v>0.00418553351047346</v>
+        <v>0.0041855263486936245</v>
       </c>
       <c r="D46" t="n">
-        <v>0.004176798530308723</v>
+        <v>0.004176791398379898</v>
       </c>
     </row>
     <row r="47">
@@ -4363,13 +4363,13 @@
         <v>48</v>
       </c>
       <c r="B47" t="n">
-        <v>10.385604</v>
+        <v>10.361146</v>
       </c>
       <c r="C47" t="n">
-        <v>9.494812423538335E-5</v>
+        <v>9.478614431213117E-5</v>
       </c>
       <c r="D47" t="n">
-        <v>9.494361694750708E-5</v>
+        <v>9.478165238929748E-5</v>
       </c>
     </row>
     <row r="48">
@@ -4377,13 +4377,13 @@
         <v>49</v>
       </c>
       <c r="B48" t="n">
-        <v>10.396463</v>
+        <v>10.371982</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0010455819420807089</v>
+        <v>0.0010458302585447665</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0010450357020079792</v>
+        <v>0.001045283759077087</v>
       </c>
     </row>
     <row r="49">
@@ -4391,13 +4391,13 @@
         <v>50</v>
       </c>
       <c r="B49" t="n">
-        <v>10.377734</v>
+        <v>10.353296</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.0018014780603748948</v>
+        <v>-0.0018015843066445658</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.0018031026734055544</v>
+        <v>-0.001803209111426618</v>
       </c>
     </row>
     <row r="50">
@@ -4405,13 +4405,13 @@
         <v>51</v>
       </c>
       <c r="B50" t="n">
-        <v>10.398502</v>
+        <v>10.374015</v>
       </c>
       <c r="C50" t="n">
-        <v>0.002001207585393683</v>
+        <v>0.002001198458925879</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0019992078369903687</v>
+        <v>0.0019991987287499846</v>
       </c>
     </row>
     <row r="51">
@@ -4419,13 +4419,13 @@
         <v>52</v>
       </c>
       <c r="B51" t="n">
-        <v>10.389617</v>
+        <v>10.36515</v>
       </c>
       <c r="C51" t="n">
-        <v>-8.544499967397812E-4</v>
+        <v>-8.545389610484788E-4</v>
       </c>
       <c r="D51" t="n">
-        <v>-8.548152472118709E-4</v>
+        <v>-8.549042876051516E-4</v>
       </c>
     </row>
     <row r="52">
@@ -4433,13 +4433,13 @@
         <v>53</v>
       </c>
       <c r="B52" t="n">
-        <v>10.440093</v>
+        <v>10.415507</v>
       </c>
       <c r="C52" t="n">
-        <v>0.00485831190889896</v>
+        <v>0.004858299204545835</v>
       </c>
       <c r="D52" t="n">
-        <v>0.004846548396752137</v>
+        <v>0.004846535753822323</v>
       </c>
     </row>
     <row r="53">
@@ -4447,13 +4447,13 @@
         <v>54</v>
       </c>
       <c r="B53" t="n">
-        <v>10.421285</v>
+        <v>10.396744</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.0018015165190580218</v>
+        <v>-0.0018014485516643086</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.0018031412014969384</v>
+        <v>-0.0018030731114402343</v>
       </c>
     </row>
     <row r="54">
@@ -4461,13 +4461,13 @@
         <v>55</v>
       </c>
       <c r="B54" t="n">
-        <v>10.402455</v>
+        <v>10.377958</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.001806878902169684</v>
+        <v>-0.0018069118562504816</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.0018085132768947965</v>
+        <v>-0.001808546290627877</v>
       </c>
     </row>
     <row r="55">
@@ -4475,13 +4475,13 @@
         <v>56</v>
       </c>
       <c r="B55" t="n">
-        <v>10.371692</v>
+        <v>10.347268</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.002957282679906026</v>
+        <v>-0.0029572291581830834</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.002961664080489257</v>
+        <v>-0.00296161040001941</v>
       </c>
     </row>
     <row r="56">
@@ -4489,13 +4489,13 @@
         <v>57</v>
       </c>
       <c r="B56" t="n">
-        <v>10.463202</v>
+        <v>10.438563</v>
       </c>
       <c r="C56" t="n">
-        <v>0.00882305413620088</v>
+        <v>0.00882310190477309</v>
       </c>
       <c r="D56" t="n">
-        <v>0.008784358436987105</v>
+        <v>0.008784405787779725</v>
       </c>
     </row>
     <row r="57">
@@ -4503,13 +4503,13 @@
         <v>58</v>
       </c>
       <c r="B57" t="n">
-        <v>10.484121</v>
+        <v>10.459432</v>
       </c>
       <c r="C57" t="n">
-        <v>0.001999292377228068</v>
+        <v>0.001999221540359697</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0019972964520724723</v>
+        <v>0.0019972257565425977</v>
       </c>
     </row>
     <row r="58">
@@ -4517,13 +4517,13 @@
         <v>59</v>
       </c>
       <c r="B58" t="n">
-        <v>10.535969</v>
+        <v>10.511158</v>
       </c>
       <c r="C58" t="n">
-        <v>0.004945383594867181</v>
+        <v>0.004945392828214823</v>
       </c>
       <c r="D58" t="n">
-        <v>0.00493319535258907</v>
+        <v>0.004933204540499059</v>
       </c>
     </row>
     <row r="59">
@@ -4531,13 +4531,13 @@
         <v>60</v>
       </c>
       <c r="B59" t="n">
-        <v>10.547955</v>
+        <v>10.523115</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0011376267337159796</v>
+        <v>0.001137553065038155</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0011369801267751</v>
+        <v>0.0011369065418067592</v>
       </c>
     </row>
     <row r="60">
@@ -4545,13 +4545,13 @@
         <v>61</v>
       </c>
       <c r="B60" t="n">
-        <v>10.53</v>
+        <v>10.505203</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.001702225692089443</v>
+        <v>-0.0017021575835673985</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.0017036761244519916</v>
+        <v>-0.0017036078997985094</v>
       </c>
     </row>
     <row r="61">
@@ -4559,13 +4559,13 @@
         <v>62</v>
       </c>
       <c r="B61" t="n">
-        <v>10.62</v>
+        <v>10.606988</v>
       </c>
       <c r="C61" t="n">
-        <v>0.008547008547008739</v>
+        <v>0.00968900838946185</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0085106896679088</v>
+        <v>0.009642370952704038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>